<commit_message>
Upload Test und plan
</commit_message>
<xml_diff>
--- a/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_gesamt.xlsx
+++ b/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_gesamt.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>Über Button "kopieren" wird Link nicht in Zwischenspeicher kopiert. Manuelles kopieren des Llinks aus dem Textfeld ist möglich.</t>
-  </si>
-  <si>
-    <t>Ergebnis wird morgen nachgetragen</t>
   </si>
   <si>
     <t>Abnahmetest durch das Team "Design"</t>
@@ -856,73 +853,6 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1096,6 +1026,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1103,12 +1039,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1323,6 +1253,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1330,12 +1266,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1463,9 +1393,76 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -1489,68 +1486,68 @@
     <tableColumn id="1" name="ID" dataDxfId="33"/>
     <tableColumn id="2" name="Testszenario" dataDxfId="32"/>
     <tableColumn id="3" name="Erwartungen" dataDxfId="31"/>
-    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="5">
+    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="30">
       <calculatedColumnFormula>Tabelle13[[#This Row],[Ergebnis Backend]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="4">
+    <tableColumn id="5" name="Kommentar Backend" dataDxfId="29">
       <calculatedColumnFormula>Tabelle13[[#This Row],[Kommentar Backend]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Ergebnis Frontend" dataDxfId="3">
+    <tableColumn id="7" name="Ergebnis Frontend" dataDxfId="28">
       <calculatedColumnFormula>Tabelle147[[#This Row],[Ergebnis Frontend]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Kommentar Frontend" dataDxfId="2">
+    <tableColumn id="8" name="Kommentar Frontend" dataDxfId="27">
       <calculatedColumnFormula>Tabelle147[[#This Row],[Kommentar Frontend]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ergebnis Design" dataDxfId="1">
+    <tableColumn id="9" name="Ergebnis Design" dataDxfId="26">
       <calculatedColumnFormula>Tabelle146[[#This Row],[Ergebnis Design]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Kommentar Design" dataDxfId="0">
+    <tableColumn id="10" name="Kommentar Design" dataDxfId="25">
       <calculatedColumnFormula>Tabelle146[[#This Row],[Kommentar Design]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ergebnis Überarbeitung" dataDxfId="30"/>
-    <tableColumn id="12" name="Kommentar Überarbeitung" dataDxfId="29"/>
+    <tableColumn id="11" name="Ergebnis Überarbeitung" dataDxfId="24"/>
+    <tableColumn id="12" name="Kommentar Überarbeitung" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="A2:E33" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle13" displayName="Tabelle13" ref="A2:E33" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="28"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="27"/>
-    <tableColumn id="3" name="Erwartungen" dataDxfId="26"/>
+    <tableColumn id="1" name="ID" dataDxfId="19"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="18"/>
+    <tableColumn id="3" name="Erwartungen" dataDxfId="17"/>
     <tableColumn id="4" name="Ergebnis Backend"/>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="25"/>
+    <tableColumn id="5" name="Kommentar Backend" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle147" displayName="Tabelle147" ref="A2:E33" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle147" displayName="Tabelle147" ref="A2:E33" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="21"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="20"/>
-    <tableColumn id="3" name="Erwartungen" dataDxfId="19"/>
-    <tableColumn id="4" name="Ergebnis Frontend" dataDxfId="18"/>
-    <tableColumn id="5" name="Kommentar Frontend" dataDxfId="17"/>
+    <tableColumn id="1" name="ID" dataDxfId="12"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="11"/>
+    <tableColumn id="3" name="Erwartungen" dataDxfId="10"/>
+    <tableColumn id="4" name="Ergebnis Frontend" dataDxfId="9"/>
+    <tableColumn id="5" name="Kommentar Frontend" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle146" displayName="Tabelle146" ref="A2:E33" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle146" displayName="Tabelle146" ref="A2:E33" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A2:E33"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="12"/>
-    <tableColumn id="3" name="Erwartungen" dataDxfId="11"/>
-    <tableColumn id="4" name="Ergebnis Design" dataDxfId="10"/>
-    <tableColumn id="5" name="Kommentar Design" dataDxfId="9"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="3"/>
+    <tableColumn id="3" name="Erwartungen" dataDxfId="2"/>
+    <tableColumn id="4" name="Ergebnis Design" dataDxfId="1"/>
+    <tableColumn id="5" name="Kommentar Design" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1880,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1973,7 +1970,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="60">
@@ -2010,7 +2009,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>Ich konnte den Fehlerfall nicht nachstellen.</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="105">
@@ -2047,7 +2048,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="60">
@@ -2084,7 +2087,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>Es wird mir jeden Wochentag diegleiche Route angezeigt.</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="45">
@@ -2121,7 +2126,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="90">
@@ -2158,7 +2165,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="60">
@@ -2195,7 +2204,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J9" s="1"/>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="30">
@@ -2232,7 +2243,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J10" s="1"/>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="75">
@@ -2269,7 +2282,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="30">
@@ -2306,7 +2321,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="30">
@@ -2343,7 +2360,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>Es wird nur die Freitagsroute angezeigt.</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="30">
@@ -2380,7 +2399,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="45">
@@ -2417,6 +2438,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v xml:space="preserve">Umlaute können (teilw.) nicht richtig angezeigt werden. Bsp: beim Sausalitos "Jumbo Cocktail f??r 5???" </v>
       </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="30">
       <c r="A16" s="13">
@@ -2452,7 +2476,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J16" s="1"/>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" ht="60">
@@ -2489,7 +2515,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>Über Button "kopieren" wird Link nicht in Zwischenspeicher kopiert. Manuelles kopieren des Llinks aus dem Textfeld ist möglich.</v>
       </c>
-      <c r="J17" s="1"/>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="45">
@@ -2526,7 +2554,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>1</v>
+      </c>
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="45">
@@ -2563,7 +2593,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J19" s="1"/>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" ht="45">
@@ -2600,7 +2632,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" ht="30">
@@ -2637,7 +2671,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" ht="45">
@@ -2674,7 +2710,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" ht="60">
@@ -2711,7 +2749,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" ht="45">
@@ -2748,7 +2788,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" ht="45">
@@ -2785,7 +2827,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J25" s="1"/>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="45">
@@ -2822,7 +2866,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J26" s="1"/>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" ht="60">
@@ -2859,7 +2905,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="30">
@@ -2896,7 +2944,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="45">
@@ -2933,7 +2983,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" ht="30">
@@ -2970,7 +3022,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" ht="30">
@@ -3007,7 +3061,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" ht="45">
@@ -3044,7 +3100,9 @@
         <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
         <v>0</v>
       </c>
-      <c r="J32" s="1"/>
+      <c r="J32" s="1">
+        <v>1</v>
+      </c>
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" ht="30">
@@ -3074,18 +3132,16 @@
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <f>Tabelle146[[#This Row],[Ergebnis Design]]</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="1" t="str">
-        <f>Tabelle146[[#This Row],[Kommentar Design]]</f>
-        <v>Ergebnis wird morgen nachgetragen</v>
-      </c>
-      <c r="J33" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
       <c r="K33" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J3:J33 D3:D33 F3:F33 H3:H33">
+  <conditionalFormatting sqref="D3:D33 F3:F33 H3:H33 J3:J33">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4198,8 +4254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4213,7 +4269,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4691,7 +4747,7 @@
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5">
       <c r="A33" s="16">
         <v>31</v>
       </c>
@@ -4701,10 +4757,10 @@
       <c r="C33" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="22" t="s">
-        <v>88</v>
-      </c>
+      <c r="D33" s="10">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D33">

</xml_diff>